<commit_message>
update productoin files rev2.1
</commit_message>
<xml_diff>
--- a/hardware/rev2/Assembly/BOM/cariboulite_r2.1_bom.xlsx
+++ b/hardware/rev2/Assembly/BOM/cariboulite_r2.1_bom.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AE1062A-7BEB-454E-A449-BA56EF1A9957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86704708-6A39-4DC0-B7E0-3F6C14D1EA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{0348B9A1-53C5-4007-8880-87B454382008}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{C4ED47CC-0B98-4CEC-852D-08EC48F07DE5}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-CaribouLite" sheetId="1" r:id="rId1"/>
@@ -1035,7 +1035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B934A17-057C-4682-9138-FA97EE258554}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808C61DC-EB85-4D06-838B-85FF2345118A}">
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>